<commit_message>
Update Students Result Individual and chart.xlsx
</commit_message>
<xml_diff>
--- a/Excel Reports/Students Result Individual and chart.xlsx
+++ b/Excel Reports/Students Result Individual and chart.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dell laptop\OneDrive\Desktop\IT\Learnig notes\Prasad assignment\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dell laptop\OneDrive\Desktop\IT\Learnig notes\Prasad assignment\VAB PROGRAMS\Excel_Programs\Excel Reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D611D8E6-336B-4EA0-85CC-CA49E6B7CF9C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{038AA318-62CF-4A4D-96E4-26371FA055F5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{9DA1665B-B63E-44EE-B4BB-0779903977F4}"/>
+    <workbookView minimized="1" xWindow="1920" yWindow="1920" windowWidth="13476" windowHeight="10620" xr2:uid="{9DA1665B-B63E-44EE-B4BB-0779903977F4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1498,22 +1498,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>65</c:v>
+                  <c:v>94</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>91</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>#N/A</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>84</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>54</c:v>
-                </c:pt>
                 <c:pt idx="4">
-                  <c:v>36</c:v>
+                  <c:v>69</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>38</c:v>
+                  <c:v>56</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>#N/A</c:v>
@@ -1651,13 +1651,13 @@
                   <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>29</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>#N/A</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>#N/A</c:v>
@@ -1666,7 +1666,7 @@
                   <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>17</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3017,10 +3017,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{650D6D6A-890B-48C0-A520-1F997A1B928A}">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AA293"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="61" workbookViewId="0">
-      <selection activeCell="W14" sqref="W14"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="W11" sqref="W11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3213,50 +3214,50 @@
         <v>PASS</v>
       </c>
       <c r="K5" s="9" t="s">
-        <v>62</v>
+        <v>73</v>
       </c>
       <c r="L5" s="10">
         <f>VLOOKUP(K5,A:H,MATCH(L4,3:3,0),0)</f>
-        <v>38</v>
+        <v>56</v>
       </c>
       <c r="N5" s="10">
         <f>VLOOKUP($K$5,$A:$H,2,0)</f>
-        <v>65</v>
+        <v>94</v>
       </c>
       <c r="O5" s="10">
         <f>VLOOKUP($K$5,$A:$H,3,0)</f>
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="P5" s="10">
         <f>VLOOKUP($K$5,$A:$H,4,0)</f>
-        <v>84</v>
+        <v>91</v>
       </c>
       <c r="Q5" s="10">
         <f>VLOOKUP($K$5,$A:$H,5,0)</f>
-        <v>54</v>
+        <v>25</v>
       </c>
       <c r="R5" s="10">
         <f>VLOOKUP($K$5,$A:$H,6,0)</f>
-        <v>36</v>
+        <v>69</v>
       </c>
       <c r="S5" s="10">
         <f>VLOOKUP($K$5,$A:$H,7,0)</f>
-        <v>38</v>
+        <v>56</v>
       </c>
       <c r="T5" s="10">
         <f>VLOOKUP($K$5,$A:$H,8,0)</f>
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="V5" s="10">
         <f>SUM(N5:T5)</f>
-        <v>323</v>
+        <v>390</v>
       </c>
       <c r="W5" s="10">
         <v>700</v>
       </c>
       <c r="X5" s="13">
         <f>V5/W5</f>
-        <v>0.46142857142857141</v>
+        <v>0.55714285714285716</v>
       </c>
       <c r="Y5" s="10" t="str">
         <f>IF(N5&lt;35,"Fail",IF(O5&lt;35,"Fail",IF(P5&lt;35,"Fail",IF(Q5&lt;35,"Fail",IF(R5&lt;35,"Fail",IF(S5&lt;35,"Fail",IF(T5&lt;35,"Fail","pass")))))))</f>
@@ -3390,7 +3391,7 @@
       </c>
       <c r="Y9" s="10" t="str">
         <f>IF(N5&lt;35,N4,IF(O5&lt;35,O4,IF(P5&lt;35,P4,IF(Q5&lt;35,Q4,IF(R5&lt;35,R4,IF(S5&lt;35,S4,IF(T5&lt;35,T4,"pass in all subjects")))))))</f>
-        <v>Science</v>
+        <v>Geography</v>
       </c>
     </row>
     <row r="10" spans="1:27" ht="23.4" x14ac:dyDescent="0.45">
@@ -3478,27 +3479,27 @@
       </c>
       <c r="N11">
         <f t="shared" ref="N11:T11" si="1">IF(N5&gt;=35,N5,NA())</f>
-        <v>65</v>
-      </c>
-      <c r="O11" t="e">
+        <v>94</v>
+      </c>
+      <c r="O11">
+        <f t="shared" si="1"/>
+        <v>37</v>
+      </c>
+      <c r="P11">
+        <f t="shared" si="1"/>
+        <v>91</v>
+      </c>
+      <c r="Q11" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="P11">
-        <f t="shared" si="1"/>
-        <v>84</v>
-      </c>
-      <c r="Q11">
-        <f t="shared" si="1"/>
-        <v>54</v>
-      </c>
       <c r="R11">
         <f t="shared" si="1"/>
-        <v>36</v>
+        <v>69</v>
       </c>
       <c r="S11">
         <f t="shared" si="1"/>
-        <v>38</v>
+        <v>56</v>
       </c>
       <c r="T11" t="e">
         <f t="shared" si="1"/>
@@ -3541,17 +3542,17 @@
         <f t="shared" ref="N12:T12" si="2">IF(N5&lt;35,N5,NA())</f>
         <v>#N/A</v>
       </c>
-      <c r="O12">
+      <c r="O12" t="e">
         <f t="shared" si="2"/>
-        <v>29</v>
+        <v>#N/A</v>
       </c>
       <c r="P12" t="e">
         <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
-      <c r="Q12" t="e">
+      <c r="Q12">
         <f t="shared" si="2"/>
-        <v>#N/A</v>
+        <v>25</v>
       </c>
       <c r="R12" t="e">
         <f t="shared" si="2"/>
@@ -3563,7 +3564,7 @@
       </c>
       <c r="T12">
         <f t="shared" si="2"/>
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:27" ht="23.4" x14ac:dyDescent="0.45">

</xml_diff>